<commit_message>
Fixing problems with templates
</commit_message>
<xml_diff>
--- a/src/assets/dna-binding_proteins.xlsx
+++ b/src/assets/dna-binding_proteins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexey/ebi_projects/faang-portal-frontend/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF7A0B4-B900-764A-8AA7-C5BA4955F2A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48CB9A1-8179-6C42-A301-3798B3FF98EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="4" xr2:uid="{58DBCFEB-F75F-A348-9496-13E962F9C8F7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="285">
   <si>
     <t>Sample Descriptor</t>
   </si>
@@ -885,6 +885,12 @@
   </si>
   <si>
     <t>ChIP Target</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Secondary Project</t>
   </si>
 </sst>
 </file>
@@ -2590,155 +2596,167 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D38584B3-9902-4E4A-AF0D-04428F33785F}">
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="39.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="39" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>70</v>
       </c>
       <c r="AB1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="X2" s="1"/>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="AA2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2749,19 +2767,19 @@
           <x14:formula1>
             <xm:f>faang_field_values!$C$1:$N$1</xm:f>
           </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
+          <xm:sqref>E2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{EA15EFDE-C0AF-3048-8AF7-BDF3DA1099D3}">
           <x14:formula1>
             <xm:f>faang_field_values!$C$2:$L$2</xm:f>
           </x14:formula1>
-          <xm:sqref>C2</xm:sqref>
+          <xm:sqref>F2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{149ADD08-0675-8F41-AA5B-1434A15C4AB5}">
           <x14:formula1>
             <xm:f>faang_field_values!$C$3:$J$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D2</xm:sqref>
+          <xm:sqref>G2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Adding adapter step field to ChIP-seq rules
</commit_message>
<xml_diff>
--- a/src/assets/dna-binding_proteins.xlsx
+++ b/src/assets/dna-binding_proteins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexey/ebi_projects/faang-portal-frontend/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B296A978-6E40-B84F-B3F2-13C23A325F55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E68B98-07DD-FB4E-A27D-C53D88A10727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{58DBCFEB-F75F-A348-9496-13E962F9C8F7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" activeTab="4" xr2:uid="{58DBCFEB-F75F-A348-9496-13E962F9C8F7}"/>
   </bookViews>
   <sheets>
     <sheet name="submission" sheetId="13" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="285">
   <si>
     <t>Sample Descriptor</t>
   </si>
@@ -888,6 +888,9 @@
   </si>
   <si>
     <t>Secondary Project</t>
+  </si>
+  <si>
+    <t>Adapter Step</t>
   </si>
 </sst>
 </file>
@@ -954,7 +957,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1274,7 +1277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{099D7B85-2870-7F44-9DA4-846DC9F871C9}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2589,10 +2592,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D38584B3-9902-4E4A-AF0D-04428F33785F}">
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2625,17 +2628,18 @@
     <col min="26" max="26" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="20" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="39.5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="39" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.83203125" customWidth="1"/>
+    <col min="30" max="30" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2721,31 +2725,34 @@
         <v>66</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>

</xml_diff>